<commit_message>
Modify scrolltoUp page, Change QR step matching SamSung devices
</commit_message>
<xml_diff>
--- a/data/userdata.xlsx
+++ b/data/userdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Auto\Checklistgolive-Refactor\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Checklistgolive-Refactor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>userKHCN</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>QmFvMjQwNzE5OTc=</t>
+  </si>
+  <si>
+    <t>BAOTG2407</t>
+  </si>
+  <si>
+    <t>002704070016694</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +449,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -449,6 +463,9 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>

</xml_diff>